<commit_message>
To be added: Achievers, authentication(RBAC), UI enhancements
</commit_message>
<xml_diff>
--- a/excel_template/student_upload_template.xlsx
+++ b/excel_template/student_upload_template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="132">
   <si>
     <t xml:space="preserve">student_id</t>
   </si>
@@ -213,10 +213,10 @@
     <t xml:space="preserve">counselling_year_of_completion</t>
   </si>
   <si>
-    <t xml:space="preserve">S2024001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rajesh Kumar</t>
+    <t xml:space="preserve">S2024009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vishnudharan</t>
   </si>
   <si>
     <t xml:space="preserve">2005-03-15</t>
@@ -228,79 +228,82 @@
     <t xml:space="preserve">OC</t>
   </si>
   <si>
+    <t xml:space="preserve">JEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234-5678-9012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APAAR001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rajesh@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC Higher Secondary School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kumar Raj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kumar@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakshmi Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teacher</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lakshmi@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10th</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABC Higher Sec</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEET</t>
   </si>
   <si>
-    <t xml:space="preserve">Biology</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9876543210</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234-5678-9012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APAAR001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rajesh@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC Higher Secondary School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kumar Raj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9876543220</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kumar@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lakshmi Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Teacher</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9876543230</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lakshmi@example.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arun Kumar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10th</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC School</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Board</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABC Higher Sec</t>
-  </si>
-  <si>
     <t xml:space="preserve">TNEA</t>
   </si>
   <si>
     <t xml:space="preserve">Govt Medical College</t>
   </si>
   <si>
-    <t xml:space="preserve">S2024002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priya Sharma</t>
+    <t xml:space="preserve">S2024012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">santhosh</t>
   </si>
   <si>
     <t xml:space="preserve">2005-06-20</t>
@@ -504,12 +507,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -707,546 +714,547 @@
   </sheetPr>
   <dimension ref="A1:BK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
+        <v>2026</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF2" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH2" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="AI2" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="AJ2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="AL2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="AM2" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="AN2" s="1" t="n">
+        <v>442</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AP2" s="1" t="n">
         <v>2024</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="AQ2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AR2" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="AS2" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="AT2" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="AU2" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="AV2" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="AW2" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="AX2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="1" t="n">
+        <v>530</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA2" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="BB2" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="BC2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="BE2" s="1" t="n">
+        <v>420</v>
+      </c>
+      <c r="BF2" s="1" t="n">
+        <v>15000</v>
+      </c>
+      <c r="BG2" s="1" t="n">
+        <v>5000</v>
+      </c>
+      <c r="BH2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BI2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BK2" s="1" t="n">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <v>2026</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="S2" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="T2" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="U2" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="V2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="W2" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB2" s="0" t="s">
+      <c r="I3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF3" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH3" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="AI3" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="AC2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="AF2" s="0" t="n">
-        <v>2022</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AH2" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="AI2" s="0" t="n">
+      <c r="AJ3" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="AJ2" s="0" t="n">
+      <c r="AK3" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="AM3" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="AN3" s="1" t="n">
+        <v>449</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AP3" s="1" t="n">
+        <v>2024</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR3" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="AS3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="AK2" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="AL2" s="0" t="n">
+      <c r="AT3" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="AU3" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="AV3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="AX3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="1" t="n">
+        <v>561</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA3" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="BB3" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="BC3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="1" t="n">
+        <v>155</v>
+      </c>
+      <c r="BE3" s="1" t="n">
+        <v>450</v>
+      </c>
+      <c r="BF3" s="1" t="n">
+        <v>8000</v>
+      </c>
+      <c r="BG3" s="1" t="n">
+        <v>2000</v>
+      </c>
+      <c r="BH3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AM2" s="0" t="n">
-        <v>87</v>
-      </c>
-      <c r="AN2" s="0" t="n">
-        <v>442</v>
-      </c>
-      <c r="AO2" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="AP2" s="0" t="n">
-        <v>2024</v>
-      </c>
-      <c r="AQ2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="AR2" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="AS2" s="0" t="n">
-        <v>80</v>
-      </c>
-      <c r="AT2" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="AU2" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="AV2" s="0" t="n">
-        <v>88</v>
-      </c>
-      <c r="AW2" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="AX2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY2" s="0" t="n">
-        <v>530</v>
-      </c>
-      <c r="AZ2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA2" s="0" t="n">
-        <v>140</v>
-      </c>
-      <c r="BB2" s="0" t="n">
-        <v>135</v>
-      </c>
-      <c r="BC2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD2" s="0" t="n">
-        <v>145</v>
-      </c>
-      <c r="BE2" s="0" t="n">
-        <v>420</v>
-      </c>
-      <c r="BF2" s="0" t="n">
-        <v>15000</v>
-      </c>
-      <c r="BG2" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="BH2" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BI2" s="0" t="n">
+      <c r="BI3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="BJ2" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="BK2" s="0" t="n">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>2024</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>99</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>103</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="W3" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="X3" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="Y3" s="0" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z3" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE3" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF3" s="0" t="n">
-        <v>2022</v>
-      </c>
-      <c r="AG3" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH3" s="0" t="n">
-        <v>90</v>
-      </c>
-      <c r="AI3" s="0" t="n">
-        <v>85</v>
-      </c>
-      <c r="AJ3" s="0" t="n">
-        <v>88</v>
-      </c>
-      <c r="AK3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="AL3" s="0" t="n">
-        <v>92</v>
-      </c>
-      <c r="AM3" s="0" t="n">
-        <v>89</v>
-      </c>
-      <c r="AN3" s="0" t="n">
-        <v>449</v>
-      </c>
-      <c r="AO3" s="0" t="s">
-        <v>111</v>
-      </c>
-      <c r="AP3" s="0" t="n">
-        <v>2024</v>
-      </c>
-      <c r="AQ3" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR3" s="0" t="n">
-        <v>88</v>
-      </c>
-      <c r="AS3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="0" t="n">
-        <v>95</v>
-      </c>
-      <c r="AU3" s="0" t="n">
-        <v>93</v>
-      </c>
-      <c r="AV3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AW3" s="0" t="n">
-        <v>97</v>
-      </c>
-      <c r="AX3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY3" s="0" t="n">
-        <v>561</v>
-      </c>
-      <c r="AZ3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA3" s="0" t="n">
-        <v>150</v>
-      </c>
-      <c r="BB3" s="0" t="n">
-        <v>145</v>
-      </c>
-      <c r="BC3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD3" s="0" t="n">
-        <v>155</v>
-      </c>
-      <c r="BE3" s="0" t="n">
-        <v>450</v>
-      </c>
-      <c r="BF3" s="0" t="n">
-        <v>8000</v>
-      </c>
-      <c r="BG3" s="0" t="n">
-        <v>2000</v>
-      </c>
-      <c r="BH3" s="0" t="s">
-        <v>89</v>
-      </c>
-      <c r="BI3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="BJ3" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="BK3" s="0" t="n">
+      <c r="BJ3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="BK3" s="1" t="n">
         <v>2030</v>
       </c>
     </row>
@@ -1275,193 +1283,193 @@
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="2" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1490,93 +1498,93 @@
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="false" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>113</v>
+      <c r="A1" s="2" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>114</v>
+      <c r="A2" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>115</v>
+      <c r="A3" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>116</v>
+      <c r="A4" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>117</v>
+      <c r="A6" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>118</v>
+      <c r="A7" s="1" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>119</v>
+      <c r="A8" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>120</v>
+      <c r="A10" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>121</v>
+      <c r="A11" s="1" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>122</v>
+      <c r="A13" s="1" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>123</v>
+      <c r="A14" s="1" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>124</v>
+      <c r="A15" s="1" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>125</v>
+      <c r="A17" s="1" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>126</v>
+      <c r="A18" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>127</v>
+      <c r="A19" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>128</v>
+      <c r="A20" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>129</v>
+      <c r="A22" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>130</v>
+      <c r="A23" s="1" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>